<commit_message>
update view bast and doc
</commit_message>
<xml_diff>
--- a/document/UAT.xlsx
+++ b/document/UAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DISBUN-APP\disbun-peminjaman-barang-iventaris\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDC8070A-6B58-440F-BFBB-908F16AA540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DB39C2-C26E-49C7-B856-6073F4465E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13760" activeTab="3" xr2:uid="{539DA2DB-6368-4B83-8F8B-4CD92101C7D5}"/>
+    <workbookView xWindow="570" yWindow="2040" windowWidth="22390" windowHeight="8690" xr2:uid="{539DA2DB-6368-4B83-8F8B-4CD92101C7D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,7 +380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45A7949-E1FA-4033-BC89-A3DAB7B25750}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
@@ -415,10 +421,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3995CA71-40DC-4489-A521-586348265950}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>